<commit_message>
update the exp results
</commit_message>
<xml_diff>
--- a/output/experiments/thesis_track_p_grid/6h-bat-Oct-track-p-grid.xlsx
+++ b/output/experiments/thesis_track_p_grid/6h-bat-Oct-track-p-grid.xlsx
@@ -271,7 +271,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-01-01-02-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-01-01-02-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-01-01-02-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_002.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-02-01-03-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -283,7 +283,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-02-01-03-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-02-01-03-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-02-01-03-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_002.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-03-01-04-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -295,7 +295,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-03-01-04-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-03-01-04-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-03-01-04-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-04-01-05-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -307,7 +307,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-04-01-05-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-04-01-05-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-04-01-05-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-05-01-06-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -319,7 +319,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-05-01-06-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-05-01-06-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-05-01-06-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-06-01-07-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -331,7 +331,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-06-01-07-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-06-01-07-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-06-01-07-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-07-01-08-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -343,7 +343,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-07-01-08-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-07-01-08-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-07-01-08-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-08-01-09-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -355,7 +355,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-08-01-09-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-08-01-09-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-08-01-09-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -367,7 +367,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -379,7 +379,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -391,7 +391,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
   <si>
     <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-by_execution-2023-09-07_001.xlsx</t>
@@ -403,7 +403,7 @@
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-by_solution-2023-09-08_001.xlsx</t>
   </si>
   <si>
-    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-minimize_cap-2023-09-07_001.xlsx</t>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-nan-nan-minimize_cap-2023-09-08_001.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1470,22 +1470,22 @@
         <v>81</v>
       </c>
       <c r="V5">
-        <v>378.8318358541226</v>
+        <v>381.7622842221533</v>
       </c>
       <c r="W5">
         <v>30.98958333333333</v>
       </c>
       <c r="X5">
-        <v>1350.4106248</v>
+        <v>1238.6643104</v>
       </c>
       <c r="Y5" t="s">
         <v>85</v>
       </c>
       <c r="Z5">
-        <v>378.8318358541226</v>
+        <v>381.7622842221533</v>
       </c>
       <c r="AA5">
-        <v>360.8318358541226</v>
+        <v>363.7622842221533</v>
       </c>
       <c r="AB5">
         <v>18</v>
@@ -1506,19 +1506,19 @@
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>0.1588754861415848</v>
+        <v>0.1600912605362297</v>
       </c>
       <c r="AI5">
-        <v>0.1588754861415848</v>
+        <v>0.1600912605362297</v>
       </c>
       <c r="AJ5">
-        <v>0.1513265990632302</v>
+        <v>0.1525429960566111</v>
       </c>
       <c r="AL5">
-        <v>110.8939531571033</v>
+        <v>100.423363368773</v>
       </c>
       <c r="AM5">
-        <v>249.9378826970193</v>
+        <v>263.5580617332523</v>
       </c>
       <c r="AO5">
         <v>62.56941176470588</v>
@@ -1527,34 +1527,34 @@
         <v>1823.944479731092</v>
       </c>
       <c r="AQ5">
-        <v>560.5129658720628</v>
+        <v>560.7096415709138</v>
       </c>
       <c r="AR5">
-        <v>2384.457445603155</v>
+        <v>2384.654121302006</v>
       </c>
       <c r="AS5">
         <v>604.9537259916899</v>
       </c>
       <c r="AT5">
-        <v>1809.73913161248</v>
+        <v>1804.585617161007</v>
       </c>
       <c r="AU5">
-        <v>5.353587442918837</v>
+        <v>4.409614257598677</v>
       </c>
       <c r="AV5">
-        <v>250.5498647811072</v>
+        <v>264.0712239680002</v>
       </c>
       <c r="AW5">
-        <v>0.6119820840879009</v>
+        <v>0.513162234747914</v>
       </c>
       <c r="AX5">
-        <v>184.8232552618388</v>
+        <v>167.3722722812883</v>
       </c>
       <c r="AY5">
-        <v>0</v>
+        <v>40.05415611619642</v>
       </c>
       <c r="AZ5">
-        <v>0</v>
+        <v>0.2191408798719717</v>
       </c>
       <c r="BA5">
         <v>-11.32715959849124</v>
@@ -2102,22 +2102,22 @@
         <v>81</v>
       </c>
       <c r="V9">
-        <v>371.3081322459453</v>
+        <v>378.7312921699576</v>
       </c>
       <c r="W9">
         <v>27.98958333333333</v>
       </c>
       <c r="X9">
-        <v>1295.9960972</v>
+        <v>1201.0645585</v>
       </c>
       <c r="Y9" t="s">
         <v>89</v>
       </c>
       <c r="Z9">
-        <v>371.3081322459453</v>
+        <v>378.7312921699576</v>
       </c>
       <c r="AA9">
-        <v>353.3081322459453</v>
+        <v>360.7312921699576</v>
       </c>
       <c r="AB9">
         <v>18</v>
@@ -2138,19 +2138,19 @@
         <v>0</v>
       </c>
       <c r="AH9">
-        <v>0.1483185819099385</v>
+        <v>0.151280509043063</v>
       </c>
       <c r="AI9">
-        <v>0.1483185819099385</v>
+        <v>0.151280509043063</v>
       </c>
       <c r="AJ9">
-        <v>0.1411285037981817</v>
+        <v>0.144090585160161</v>
       </c>
       <c r="AL9">
-        <v>106.5589862281232</v>
+        <v>103.8987204790237</v>
       </c>
       <c r="AM9">
-        <v>246.7491460178221</v>
+        <v>257.1597640051947</v>
       </c>
       <c r="AO9">
         <v>69.49013770003722</v>
@@ -2159,34 +2159,34 @@
         <v>1897.080720803875</v>
       </c>
       <c r="AQ9">
-        <v>606.3691333176376</v>
+        <v>606.4228340536064</v>
       </c>
       <c r="AR9">
-        <v>2503.449854121513</v>
+        <v>2503.503554857481</v>
       </c>
       <c r="AS9">
         <v>747.2553716424334</v>
       </c>
       <c r="AT9">
-        <v>1790.140456522292</v>
+        <v>1785.347397625189</v>
       </c>
       <c r="AU9">
-        <v>9.030903313973955</v>
+        <v>6.807237924860658</v>
       </c>
       <c r="AV9">
-        <v>247.8780811967644</v>
+        <v>258.0489082644798</v>
       </c>
       <c r="AW9">
-        <v>1.128935178942237</v>
+        <v>0.8891442592851279</v>
       </c>
       <c r="AX9">
-        <v>177.5983103802052</v>
+        <v>173.1645341317061</v>
       </c>
       <c r="AY9">
-        <v>0</v>
+        <v>54.01400200883849</v>
       </c>
       <c r="AZ9">
-        <v>0</v>
+        <v>0.3271923142607898</v>
       </c>
       <c r="BA9">
         <v>-12.19819991079334</v>
@@ -2734,22 +2734,22 @@
         <v>81</v>
       </c>
       <c r="V13">
-        <v>323.5723865595441</v>
+        <v>319.8925843792476</v>
       </c>
       <c r="W13">
         <v>30.98958333333333</v>
       </c>
       <c r="X13">
-        <v>1330.0328642</v>
+        <v>1219.1102593</v>
       </c>
       <c r="Y13" t="s">
         <v>93</v>
       </c>
       <c r="Z13">
-        <v>323.5723865595441</v>
+        <v>319.8925843792476</v>
       </c>
       <c r="AA13">
-        <v>305.5723865595441</v>
+        <v>301.8925843792476</v>
       </c>
       <c r="AB13">
         <v>18</v>
@@ -2770,19 +2770,19 @@
         <v>0</v>
       </c>
       <c r="AH13">
-        <v>0.1365784413450851</v>
+        <v>0.1350252134828842</v>
       </c>
       <c r="AI13">
-        <v>0.1365784413450851</v>
+        <v>0.1350252134828842</v>
       </c>
       <c r="AJ13">
-        <v>0.1289807227314817</v>
+        <v>0.1274274948692808</v>
       </c>
       <c r="AL13">
-        <v>108.6235597207575</v>
+        <v>94.14891521222496</v>
       </c>
       <c r="AM13">
-        <v>196.9488268387866</v>
+        <v>208.2638731769835</v>
       </c>
       <c r="AO13">
         <v>61.60134453781513</v>
@@ -2800,25 +2800,25 @@
         <v>944.9298545577608</v>
       </c>
       <c r="AT13">
-        <v>1492.582067913237</v>
+        <v>1469.804033549719</v>
       </c>
       <c r="AU13">
-        <v>42.6822232898523</v>
+        <v>22.61344177428888</v>
       </c>
       <c r="AV13">
-        <v>202.5799944505576</v>
+        <v>210.9446171702643</v>
       </c>
       <c r="AW13">
-        <v>5.631167611771006</v>
+        <v>2.680743993280815</v>
       </c>
       <c r="AX13">
-        <v>181.0392662012625</v>
+        <v>156.9148586870416</v>
       </c>
       <c r="AY13">
-        <v>0</v>
+        <v>95.08190639471097</v>
       </c>
       <c r="AZ13">
-        <v>0</v>
+        <v>0.5202040099608033</v>
       </c>
       <c r="BA13">
         <v>-16.17920982126445</v>
@@ -3366,22 +3366,22 @@
         <v>81</v>
       </c>
       <c r="V17">
-        <v>331.1741813942341</v>
+        <v>328.3788769401734</v>
       </c>
       <c r="W17">
         <v>29.98958333333333</v>
       </c>
       <c r="X17">
-        <v>1584.2451851</v>
+        <v>1462.5820843</v>
       </c>
       <c r="Y17" t="s">
         <v>97</v>
       </c>
       <c r="Z17">
-        <v>331.1741813942341</v>
+        <v>328.3788769401734</v>
       </c>
       <c r="AA17">
-        <v>313.1741813942341</v>
+        <v>310.3788769401734</v>
       </c>
       <c r="AB17">
         <v>18</v>
@@ -3402,19 +3402,19 @@
         <v>0</v>
       </c>
       <c r="AH17">
-        <v>0.1276129158245017</v>
+        <v>0.1265334091252801</v>
       </c>
       <c r="AI17">
-        <v>0.1276129158245017</v>
+        <v>0.1265334091252801</v>
       </c>
       <c r="AJ17">
-        <v>0.1206768905728635</v>
+        <v>0.119597514266641</v>
       </c>
       <c r="AL17">
-        <v>108.7013935981012</v>
+        <v>93.06812538604369</v>
       </c>
       <c r="AM17">
-        <v>204.4727877961329</v>
+        <v>217.3107515541297</v>
       </c>
       <c r="AO17">
         <v>79.39423410906565</v>
@@ -3423,28 +3423,28 @@
         <v>1901.742151302541</v>
       </c>
       <c r="AQ17">
-        <v>693.404109987169</v>
+        <v>693.4528980543224</v>
       </c>
       <c r="AR17">
-        <v>2595.146261289709</v>
+        <v>2595.195049356863</v>
       </c>
       <c r="AS17">
         <v>1094.388561628032</v>
       </c>
       <c r="AT17">
-        <v>1541.462857097989</v>
+        <v>1527.011154796215</v>
       </c>
       <c r="AU17">
-        <v>14.84169061580886</v>
+        <v>6.115309273527662</v>
       </c>
       <c r="AV17">
-        <v>206.6951118256528</v>
+        <v>218.0670793198073</v>
       </c>
       <c r="AW17">
-        <v>2.222324029519883</v>
+        <v>0.7563277656775866</v>
       </c>
       <c r="AX17">
-        <v>181.1689893301687</v>
+        <v>155.1135423100728</v>
       </c>
       <c r="AY17">
         <v>0</v>
@@ -3998,22 +3998,22 @@
         <v>81</v>
       </c>
       <c r="V21">
-        <v>336.7556753716689</v>
+        <v>331.9143485514842</v>
       </c>
       <c r="W21">
         <v>30.98958333333333</v>
       </c>
       <c r="X21">
-        <v>1579.4276043</v>
+        <v>1511.2594947</v>
       </c>
       <c r="Y21" t="s">
         <v>101</v>
       </c>
       <c r="Z21">
-        <v>336.7556753716689</v>
+        <v>331.9143485514842</v>
       </c>
       <c r="AA21">
-        <v>318.7556753716689</v>
+        <v>313.9143485514842</v>
       </c>
       <c r="AB21">
         <v>18</v>
@@ -4034,19 +4034,19 @@
         <v>0</v>
       </c>
       <c r="AH21">
-        <v>0.1314053442531573</v>
+        <v>0.1295202985453993</v>
       </c>
       <c r="AI21">
-        <v>0.1314053442531573</v>
+        <v>0.1295202985453993</v>
       </c>
       <c r="AJ21">
-        <v>0.1243815689479711</v>
+        <v>0.1224963015895835</v>
       </c>
       <c r="AL21">
-        <v>106.4060359165518</v>
+        <v>89.44986790154844</v>
       </c>
       <c r="AM21">
-        <v>212.349639455117</v>
+        <v>224.5182362881832</v>
       </c>
       <c r="AO21">
         <v>80.73680672268908</v>
@@ -4055,34 +4055,34 @@
         <v>1862.336656134451</v>
       </c>
       <c r="AQ21">
-        <v>700.3876933630587</v>
+        <v>700.306823529412</v>
       </c>
       <c r="AR21">
-        <v>2562.724349497509</v>
+        <v>2562.643479663862</v>
       </c>
       <c r="AS21">
         <v>998.2962822620709</v>
       </c>
       <c r="AT21">
-        <v>1618.787222142834</v>
+        <v>1595.896016282618</v>
       </c>
       <c r="AU21">
-        <v>28.60521592611861</v>
+        <v>11.32613513684279</v>
       </c>
       <c r="AV21">
-        <v>216.4964892214551</v>
+        <v>225.8428845473684</v>
       </c>
       <c r="AW21">
-        <v>4.146849766338057</v>
+        <v>1.324648259185148</v>
       </c>
       <c r="AX21">
-        <v>177.343393194253</v>
+        <v>149.0831131692474</v>
       </c>
       <c r="AY21">
-        <v>0</v>
+        <v>9.825354026807531</v>
       </c>
       <c r="AZ21">
-        <v>0</v>
+        <v>0.05375563824742705</v>
       </c>
       <c r="BA21">
         <v>-14.6629732887026</v>
@@ -4630,22 +4630,22 @@
         <v>81</v>
       </c>
       <c r="V25">
-        <v>309.6168070412068</v>
+        <v>311.1362173684662</v>
       </c>
       <c r="W25">
         <v>29.98958333333333</v>
       </c>
       <c r="X25">
-        <v>1242.084621399999</v>
+        <v>1202.5276552</v>
       </c>
       <c r="Y25" t="s">
         <v>105</v>
       </c>
       <c r="Z25">
-        <v>309.6168070412068</v>
+        <v>311.1362173684662</v>
       </c>
       <c r="AA25">
-        <v>291.6168070412068</v>
+        <v>293.1362173684662</v>
       </c>
       <c r="AB25">
         <v>18</v>
@@ -4666,19 +4666,19 @@
         <v>0</v>
       </c>
       <c r="AH25">
-        <v>0.1392495640639949</v>
+        <v>0.1399289434667034</v>
       </c>
       <c r="AI25">
-        <v>0.1392495640639949</v>
+        <v>0.1399289434667034</v>
       </c>
       <c r="AJ25">
-        <v>0.1311540986494887</v>
+        <v>0.1318337078695635</v>
       </c>
       <c r="AL25">
-        <v>106.0479950548862</v>
+        <v>96.84935292972744</v>
       </c>
       <c r="AM25">
-        <v>185.5688119863207</v>
+        <v>197.5573968366753</v>
       </c>
       <c r="AO25">
         <v>62.55505383813824</v>
@@ -4687,34 +4687,34 @@
         <v>1678.163552344566</v>
       </c>
       <c r="AQ25">
-        <v>545.3034230990072</v>
+        <v>545.3665455761844</v>
       </c>
       <c r="AR25">
-        <v>2223.466975443574</v>
+        <v>2223.53009792075</v>
       </c>
       <c r="AS25">
         <v>840.6148316061417</v>
       </c>
       <c r="AT25">
-        <v>1461.203479451276</v>
+        <v>1427.043869798723</v>
       </c>
       <c r="AU25">
-        <v>52.69095608971679</v>
+        <v>17.24144434714563</v>
       </c>
       <c r="AV25">
-        <v>193.4691873176189</v>
+        <v>199.9453416704439</v>
       </c>
       <c r="AW25">
-        <v>7.900375331298196</v>
+        <v>2.38794483376855</v>
       </c>
       <c r="AX25">
-        <v>176.7466584248103</v>
+        <v>161.4155882162124</v>
       </c>
       <c r="AY25">
-        <v>0</v>
+        <v>224.7315877649988</v>
       </c>
       <c r="AZ25">
-        <v>0</v>
+        <v>1.270532397936547</v>
       </c>
       <c r="BA25">
         <v>-12.67179709055496</v>
@@ -5262,22 +5262,22 @@
         <v>81</v>
       </c>
       <c r="V29">
-        <v>252.829854737865</v>
+        <v>223.2638435420032</v>
       </c>
       <c r="W29">
         <v>30.98958333333333</v>
       </c>
       <c r="X29">
-        <v>1232.2678752</v>
+        <v>1169.5332397</v>
       </c>
       <c r="Y29" t="s">
         <v>109</v>
       </c>
       <c r="Z29">
-        <v>252.829854737865</v>
+        <v>223.2638435420032</v>
       </c>
       <c r="AA29">
-        <v>234.829854737865</v>
+        <v>205.2638435420032</v>
       </c>
       <c r="AB29">
         <v>18</v>
@@ -5298,19 +5298,19 @@
         <v>0</v>
       </c>
       <c r="AH29">
-        <v>0.1177513424974344</v>
+        <v>0.1039746882379047</v>
       </c>
       <c r="AI29">
-        <v>0.1177513424974344</v>
+        <v>0.1039746882379047</v>
       </c>
       <c r="AJ29">
-        <v>0.1093681388320629</v>
+        <v>0.09559203048826245</v>
       </c>
       <c r="AL29">
-        <v>105.8134854485876</v>
+        <v>64.44381977257362</v>
       </c>
       <c r="AM29">
-        <v>129.0163692892774</v>
+        <v>141.5501548826628</v>
       </c>
       <c r="AO29">
         <v>58.69714285714286</v>
@@ -5319,34 +5319,34 @@
         <v>1588.554786151262</v>
       </c>
       <c r="AQ29">
-        <v>558.5957208026069</v>
+        <v>558.7355527353792</v>
       </c>
       <c r="AR29">
-        <v>2147.150506953869</v>
+        <v>2147.290338886641</v>
       </c>
       <c r="AS29">
         <v>1167.710296098818</v>
       </c>
       <c r="AT29">
-        <v>1108.481389353206</v>
+        <v>1033.1591836436</v>
       </c>
       <c r="AU29">
-        <v>103.6238912631243</v>
+        <v>31.73312956314376</v>
       </c>
       <c r="AV29">
-        <v>144.7389549494254</v>
+        <v>145.0147040711629</v>
       </c>
       <c r="AW29">
-        <v>15.722585660148</v>
+        <v>3.46454918850011</v>
       </c>
       <c r="AX29">
-        <v>176.3558090809794</v>
+        <v>107.4063662876227</v>
       </c>
       <c r="AY29">
-        <v>0</v>
+        <v>133.4519858267323</v>
       </c>
       <c r="AZ29">
-        <v>0</v>
+        <v>0.7301311132331286</v>
       </c>
       <c r="BA29">
         <v>-14.06128093638941</v>
@@ -5894,22 +5894,22 @@
         <v>81</v>
       </c>
       <c r="V33">
-        <v>258.410783430172</v>
+        <v>233.3653695316492</v>
       </c>
       <c r="W33">
         <v>30.98958333333333</v>
       </c>
       <c r="X33">
-        <v>1139.655518400001</v>
+        <v>1086.3745479</v>
       </c>
       <c r="Y33" t="s">
         <v>113</v>
       </c>
       <c r="Z33">
-        <v>258.410783430172</v>
+        <v>233.3653695316492</v>
       </c>
       <c r="AA33">
-        <v>240.4107834301721</v>
+        <v>215.3653695316492</v>
       </c>
       <c r="AB33">
         <v>18</v>
@@ -5930,19 +5930,19 @@
         <v>0</v>
       </c>
       <c r="AH33">
-        <v>0.1204150980629855</v>
+        <v>0.1087443545646453</v>
       </c>
       <c r="AI33">
-        <v>0.1204150980629855</v>
+        <v>0.1087443545646453</v>
       </c>
       <c r="AJ33">
-        <v>0.112027399467894</v>
+        <v>0.1003566559695538</v>
       </c>
       <c r="AL33">
-        <v>104.352103293657</v>
+        <v>65.956972776347</v>
       </c>
       <c r="AM33">
-        <v>136.0586801365151</v>
+        <v>149.9350775801196</v>
       </c>
       <c r="AO33">
         <v>54.59899159663865</v>
@@ -5951,7 +5951,7 @@
         <v>1615.704738151263</v>
       </c>
       <c r="AQ33">
-        <v>530.295120562511</v>
+        <v>530.2951205625106</v>
       </c>
       <c r="AR33">
         <v>2145.999858713773</v>
@@ -5960,25 +5960,25 @@
         <v>1110.784748030245</v>
       </c>
       <c r="AT33">
-        <v>1141.090202355252</v>
+        <v>1071.905169927031</v>
       </c>
       <c r="AU33">
-        <v>79.78300271518238</v>
+        <v>15.61085430927645</v>
       </c>
       <c r="AV33">
-        <v>148.8092781058309</v>
+        <v>151.7337745682448</v>
       </c>
       <c r="AW33">
-        <v>12.75059796931574</v>
+        <v>1.798696988125188</v>
       </c>
       <c r="AX33">
-        <v>173.920172156095</v>
+        <v>109.9282879605784</v>
       </c>
       <c r="AY33">
-        <v>1.4210854715202E-14</v>
+        <v>96.26572638098139</v>
       </c>
       <c r="AZ33">
-        <v>7.774921526215518E-17</v>
+        <v>0.5266808248173875</v>
       </c>
       <c r="BA33">
         <v>-9.013058559235162</v>
@@ -6526,22 +6526,22 @@
         <v>81</v>
       </c>
       <c r="V37">
-        <v>291.7117582021184</v>
+        <v>284.9811300356272</v>
       </c>
       <c r="W37">
         <v>29.98958333333333</v>
       </c>
       <c r="X37">
-        <v>1285.328403699999</v>
+        <v>1218.0763376</v>
       </c>
       <c r="Y37" t="s">
         <v>117</v>
       </c>
       <c r="Z37">
-        <v>291.7117582021184</v>
+        <v>284.9811300356272</v>
       </c>
       <c r="AA37">
-        <v>273.7117582021184</v>
+        <v>266.9811300356272</v>
       </c>
       <c r="AB37">
         <v>18</v>
@@ -6562,19 +6562,19 @@
         <v>0</v>
       </c>
       <c r="AH37">
-        <v>0.1304802762960188</v>
+        <v>0.1274697215339408</v>
       </c>
       <c r="AI37">
-        <v>0.1304802762960188</v>
+        <v>0.1274697215339408</v>
       </c>
       <c r="AJ37">
-        <v>0.1224290239645957</v>
+        <v>0.1194184692025177</v>
       </c>
       <c r="AL37">
-        <v>106.248898163098</v>
+        <v>87.03783460116286</v>
       </c>
       <c r="AM37">
-        <v>167.4628600390203</v>
+        <v>180.1116038895606</v>
       </c>
       <c r="AO37">
         <v>64.35567905522751</v>
@@ -6583,7 +6583,7 @@
         <v>1640.910548940604</v>
       </c>
       <c r="AQ37">
-        <v>594.7664934678285</v>
+        <v>594.7664934678277</v>
       </c>
       <c r="AR37">
         <v>2235.677042408432</v>
@@ -6592,25 +6592,25 @@
         <v>987.6318419771399</v>
       </c>
       <c r="AT37">
-        <v>1303.880840012598</v>
+        <v>1275.759182717254</v>
       </c>
       <c r="AU37">
-        <v>30.00263029589359</v>
+        <v>7.246192519998683</v>
       </c>
       <c r="AV37">
-        <v>172.1694802354543</v>
+        <v>181.0260442021478</v>
       </c>
       <c r="AW37">
-        <v>4.70662019643399</v>
+        <v>0.9144403125872189</v>
       </c>
       <c r="AX37">
-        <v>177.0814969384967</v>
+        <v>145.0630576686048</v>
       </c>
       <c r="AY37">
-        <v>0</v>
+        <v>29.77037532414831</v>
       </c>
       <c r="AZ37">
-        <v>0</v>
+        <v>0.1683084550962807</v>
       </c>
       <c r="BA37">
         <v>-11.5999000202558</v>
@@ -7158,22 +7158,22 @@
         <v>81</v>
       </c>
       <c r="V41">
-        <v>371.0884886405262</v>
+        <v>359.5342253400781</v>
       </c>
       <c r="W41">
         <v>30.98958333333333</v>
       </c>
       <c r="X41">
-        <v>1749.0054482</v>
+        <v>1603.303729</v>
       </c>
       <c r="Y41" t="s">
         <v>121</v>
       </c>
       <c r="Z41">
-        <v>371.0884886405262</v>
+        <v>359.5342253400781</v>
       </c>
       <c r="AA41">
-        <v>353.0884886405262</v>
+        <v>341.5342253400781</v>
       </c>
       <c r="AB41">
         <v>18</v>
@@ -7194,19 +7194,19 @@
         <v>0</v>
       </c>
       <c r="AH41">
-        <v>0.1377822058801722</v>
+        <v>0.1334921997668373</v>
       </c>
       <c r="AI41">
-        <v>0.1377822058801722</v>
+        <v>0.1334921997668373</v>
       </c>
       <c r="AJ41">
-        <v>0.1310989489704016</v>
+        <v>0.1268089428570668</v>
       </c>
       <c r="AL41">
-        <v>108.1378678442093</v>
+        <v>83.26105551668992</v>
       </c>
       <c r="AM41">
-        <v>244.9506207963169</v>
+        <v>258.5388161535467</v>
       </c>
       <c r="AO41">
         <v>91.74050420168068</v>
@@ -7215,7 +7215,7 @@
         <v>1861.262727529411</v>
       </c>
       <c r="AQ41">
-        <v>832.0349031040994</v>
+        <v>832.0349031040995</v>
       </c>
       <c r="AR41">
         <v>2693.29763063351</v>
@@ -7224,25 +7224,25 @@
         <v>932.8271981736434</v>
       </c>
       <c r="AT41">
-        <v>1789.717774479305</v>
+        <v>1784.609881155756</v>
       </c>
       <c r="AU41">
-        <v>3.043577363570798</v>
+        <v>1.908148349886507</v>
       </c>
       <c r="AV41">
-        <v>245.397137215943</v>
+        <v>258.8310040101808</v>
       </c>
       <c r="AW41">
-        <v>0.4465164196260386</v>
+        <v>0.2921878566340159</v>
       </c>
       <c r="AX41">
-        <v>180.2297797403488</v>
+        <v>138.7684258611499</v>
       </c>
       <c r="AY41">
-        <v>0</v>
+        <v>48.55433448145752</v>
       </c>
       <c r="AZ41">
-        <v>0</v>
+        <v>0.2656463301585349</v>
       </c>
       <c r="BA41">
         <v>-12.71181636181905</v>
@@ -7790,22 +7790,22 @@
         <v>81</v>
       </c>
       <c r="V45">
-        <v>407.2004744779421</v>
+        <v>396.2144451703995</v>
       </c>
       <c r="W45">
         <v>29.98958333333333</v>
       </c>
       <c r="X45">
-        <v>1458.429696800001</v>
+        <v>1358.5385934</v>
       </c>
       <c r="Y45" t="s">
         <v>125</v>
       </c>
       <c r="Z45">
-        <v>407.2004744779421</v>
+        <v>396.2144451703995</v>
       </c>
       <c r="AA45">
-        <v>389.2004744779421</v>
+        <v>378.2144451703995</v>
       </c>
       <c r="AB45">
         <v>18</v>
@@ -7826,19 +7826,19 @@
         <v>0</v>
       </c>
       <c r="AH45">
-        <v>0.1618682297377508</v>
+        <v>0.1575011201017935</v>
       </c>
       <c r="AI45">
-        <v>0.1618682297377508</v>
+        <v>0.1575011201017935</v>
       </c>
       <c r="AJ45">
-        <v>0.1547129626938825</v>
+        <v>0.1503458530579253</v>
       </c>
       <c r="AL45">
-        <v>122.26998</v>
+        <v>102.2603489709766</v>
       </c>
       <c r="AM45">
-        <v>266.9304944779421</v>
+        <v>276.0866970513032</v>
       </c>
       <c r="AO45">
         <v>79.36088919763807</v>
@@ -7847,7 +7847,7 @@
         <v>1761.196290656481</v>
       </c>
       <c r="AQ45">
-        <v>754.43308972078</v>
+        <v>754.4330897207806</v>
       </c>
       <c r="AR45">
         <v>2515.629380377261</v>
@@ -7856,25 +7856,25 @@
         <v>626.1831707214252</v>
       </c>
       <c r="AT45">
-        <v>1926.452532257326</v>
+        <v>1920.633769695537</v>
       </c>
       <c r="AU45">
-        <v>11.91275710870359</v>
+        <v>9.55135447016875</v>
       </c>
       <c r="AV45">
-        <v>268.5760643200935</v>
+        <v>277.4947509882299</v>
       </c>
       <c r="AW45">
-        <v>1.645569842151344</v>
+        <v>1.408053936926675</v>
       </c>
       <c r="AX45">
-        <v>203.7833</v>
+        <v>170.4339149516277</v>
       </c>
       <c r="AY45">
-        <v>3.552713678800501E-15</v>
+        <v>23.45441960430264</v>
       </c>
       <c r="AZ45">
-        <v>2.008546228146833E-17</v>
+        <v>0.1326008518803594</v>
       </c>
       <c r="BA45">
         <v>-61.13808536617337</v>
@@ -8326,22 +8326,22 @@
         <v>81</v>
       </c>
       <c r="V49">
-        <v>344.7856503110191</v>
+        <v>353.5612346795531</v>
       </c>
       <c r="W49">
         <v>29.98958333333333</v>
       </c>
       <c r="X49">
-        <v>1122.2175209</v>
+        <v>1102.9779828</v>
       </c>
       <c r="Y49" t="s">
         <v>129</v>
       </c>
       <c r="Z49">
-        <v>344.7856503110191</v>
+        <v>353.5612346795531</v>
       </c>
       <c r="AA49">
-        <v>326.7856503110191</v>
+        <v>335.5612346795531</v>
       </c>
       <c r="AB49">
         <v>18</v>
@@ -8362,19 +8362,19 @@
         <v>0</v>
       </c>
       <c r="AH49">
-        <v>0.1670691507571029</v>
+        <v>0.1713214432365774</v>
       </c>
       <c r="AI49">
-        <v>0.1670691507571029</v>
+        <v>0.1713214432365774</v>
       </c>
       <c r="AJ49">
-        <v>0.1583470803608578</v>
+        <v>0.1625993728403323</v>
       </c>
       <c r="AL49">
         <v>106.6033800307256</v>
       </c>
       <c r="AM49">
-        <v>220.1822702802935</v>
+        <v>229.4392872459554</v>
       </c>
       <c r="AO49">
         <v>58.68704411253908</v>
@@ -8392,25 +8392,25 @@
         <v>475.3545887162526</v>
       </c>
       <c r="AT49">
-        <v>1648.942828789293</v>
+        <v>1634.710088034392</v>
       </c>
       <c r="AU49">
-        <v>34.96028882029493</v>
+        <v>22.84944035846</v>
       </c>
       <c r="AV49">
-        <v>224.8280596562575</v>
+        <v>232.4805308339622</v>
       </c>
       <c r="AW49">
-        <v>4.645789375964013</v>
+        <v>3.041243588006854</v>
       </c>
       <c r="AX49">
         <v>177.6723000512094</v>
       </c>
       <c r="AY49">
-        <v>0</v>
+        <v>85.15572851986794</v>
       </c>
       <c r="AZ49">
-        <v>0</v>
+        <v>0.4814325971279066</v>
       </c>
       <c r="BA49">
         <v>-16.59457687080194</v>

</xml_diff>